<commit_message>
fix date format in project tab
</commit_message>
<xml_diff>
--- a/data/GEP00004/GEP00004_ARID1B.xlsx
+++ b/data/GEP00004/GEP00004_ARID1B.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smith04\Desktop\NGS Submission\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="-40" yWindow="8180" windowWidth="16380" windowHeight="8200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -21,8 +16,11 @@
     <sheet name="Plate" sheetId="7" r:id="rId7"/>
     <sheet name="SequencingLibrary" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -972,8 +970,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1003,6 +1001,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1021,10 +1035,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1042,8 +1058,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1102,7 +1121,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1137,7 +1156,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1314,7 +1333,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1322,24 +1341,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="5" width="11.5703125"/>
-    <col min="6" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" customWidth="1"/>
-    <col min="10" max="1025" width="11.5703125"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="6" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="9" max="9" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1384,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -1387,8 +1403,8 @@
       <c r="F2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="1">
-        <v>42950</v>
+      <c r="G2" s="11">
+        <v>20170803</v>
       </c>
       <c r="H2" t="s">
         <v>58</v>
@@ -1396,6 +1412,9 @@
       <c r="I2" t="s">
         <v>66</v>
       </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1404,6 +1423,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1411,20 +1435,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="11.5703125"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="1025" width="11.5703125"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -1488,16 +1509,21 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="G3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1505,20 +1531,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="1025" width="11.5703125"/>
+    <col min="1" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1541,7 +1566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>187</v>
       </c>
@@ -1564,7 +1589,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>187</v>
       </c>
@@ -1594,6 +1619,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1601,20 +1631,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1635,6 +1663,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1642,30 +1675,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="7" width="11.5703125"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="16" width="14.85546875" customWidth="1"/>
-    <col min="17" max="18" width="31.7109375" customWidth="1"/>
-    <col min="19" max="21" width="14.85546875" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" customWidth="1"/>
-    <col min="23" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="11" max="14" width="14.1640625" customWidth="1"/>
+    <col min="15" max="16" width="14.83203125" customWidth="1"/>
+    <col min="17" max="18" width="31.6640625" customWidth="1"/>
+    <col min="19" max="21" width="14.83203125" customWidth="1"/>
+    <col min="22" max="22" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1718,7 +1749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>179</v>
       </c>
@@ -1770,7 +1801,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>180</v>
       </c>
@@ -1822,7 +1853,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="K6" s="2"/>
     </row>
   </sheetData>
@@ -1832,6 +1863,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1839,24 +1875,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="6" width="11.5703125"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="1" max="2" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="1025" width="11.5703125"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1888,7 +1921,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -1908,7 +1941,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -1940,7 +1973,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -1972,7 +2005,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>178</v>
       </c>
@@ -2004,7 +2037,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>178</v>
       </c>
@@ -2036,7 +2069,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>178</v>
       </c>
@@ -2068,7 +2101,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -2100,7 +2133,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>178</v>
       </c>
@@ -2132,7 +2165,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -2164,7 +2197,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>178</v>
       </c>
@@ -2196,7 +2229,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>178</v>
       </c>
@@ -2216,7 +2249,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -2248,7 +2281,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>178</v>
       </c>
@@ -2280,7 +2313,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>178</v>
       </c>
@@ -2312,7 +2345,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>178</v>
       </c>
@@ -2344,7 +2377,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>178</v>
       </c>
@@ -2376,7 +2409,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>178</v>
       </c>
@@ -2408,7 +2441,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>178</v>
       </c>
@@ -2440,7 +2473,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>178</v>
       </c>
@@ -2472,7 +2505,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>178</v>
       </c>
@@ -2504,7 +2537,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>178</v>
       </c>
@@ -2536,7 +2569,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>178</v>
       </c>
@@ -2568,7 +2601,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>178</v>
       </c>
@@ -2588,7 +2621,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>178</v>
       </c>
@@ -2620,7 +2653,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>178</v>
       </c>
@@ -2652,7 +2685,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>178</v>
       </c>
@@ -2684,7 +2717,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>178</v>
       </c>
@@ -2716,7 +2749,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>178</v>
       </c>
@@ -2748,7 +2781,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>178</v>
       </c>
@@ -2780,7 +2813,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>178</v>
       </c>
@@ -2812,7 +2845,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>178</v>
       </c>
@@ -2844,7 +2877,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>178</v>
       </c>
@@ -2876,7 +2909,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>178</v>
       </c>
@@ -2908,7 +2941,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>178</v>
       </c>
@@ -2940,7 +2973,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>178</v>
       </c>
@@ -2960,7 +2993,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>178</v>
       </c>
@@ -2992,7 +3025,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>178</v>
       </c>
@@ -3024,7 +3057,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -3056,7 +3089,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>178</v>
       </c>
@@ -3088,7 +3121,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -3120,7 +3153,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>178</v>
       </c>
@@ -3152,7 +3185,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>178</v>
       </c>
@@ -3184,7 +3217,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>178</v>
       </c>
@@ -3216,7 +3249,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>178</v>
       </c>
@@ -3248,7 +3281,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -3280,7 +3313,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>178</v>
       </c>
@@ -3312,7 +3345,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>178</v>
       </c>
@@ -3332,7 +3365,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>178</v>
       </c>
@@ -3364,7 +3397,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>178</v>
       </c>
@@ -3396,7 +3429,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>178</v>
       </c>
@@ -3428,7 +3461,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>178</v>
       </c>
@@ -3460,7 +3493,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>178</v>
       </c>
@@ -3492,7 +3525,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>178</v>
       </c>
@@ -3524,7 +3557,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>178</v>
       </c>
@@ -3556,7 +3589,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>178</v>
       </c>
@@ -3588,7 +3621,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>178</v>
       </c>
@@ -3620,7 +3653,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>178</v>
       </c>
@@ -3652,7 +3685,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>178</v>
       </c>
@@ -3684,7 +3717,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>178</v>
       </c>
@@ -3704,7 +3737,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>178</v>
       </c>
@@ -3736,7 +3769,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>178</v>
       </c>
@@ -3768,7 +3801,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>178</v>
       </c>
@@ -3800,7 +3833,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>178</v>
       </c>
@@ -3832,7 +3865,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>178</v>
       </c>
@@ -3864,7 +3897,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>178</v>
       </c>
@@ -3896,7 +3929,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>178</v>
       </c>
@@ -3928,7 +3961,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>178</v>
       </c>
@@ -3960,7 +3993,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>178</v>
       </c>
@@ -3992,7 +4025,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>178</v>
       </c>
@@ -4024,7 +4057,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -4056,7 +4089,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>178</v>
       </c>
@@ -4076,7 +4109,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>178</v>
       </c>
@@ -4108,7 +4141,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>178</v>
       </c>
@@ -4140,7 +4173,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>178</v>
       </c>
@@ -4172,7 +4205,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>178</v>
       </c>
@@ -4204,7 +4237,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>178</v>
       </c>
@@ -4236,7 +4269,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>178</v>
       </c>
@@ -4268,7 +4301,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>178</v>
       </c>
@@ -4300,7 +4333,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>178</v>
       </c>
@@ -4332,7 +4365,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -4364,7 +4397,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>178</v>
       </c>
@@ -4396,7 +4429,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>178</v>
       </c>
@@ -4428,7 +4461,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>178</v>
       </c>
@@ -4448,7 +4481,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>178</v>
       </c>
@@ -4480,7 +4513,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>178</v>
       </c>
@@ -4512,7 +4545,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
         <v>178</v>
       </c>
@@ -4544,7 +4577,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>178</v>
       </c>
@@ -4576,7 +4609,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>178</v>
       </c>
@@ -4608,7 +4641,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>178</v>
       </c>
@@ -4640,7 +4673,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -4672,7 +4705,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>178</v>
       </c>
@@ -4704,7 +4737,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>178</v>
       </c>
@@ -4736,7 +4769,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>178</v>
       </c>
@@ -4768,7 +4801,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
         <v>178</v>
       </c>
@@ -4800,7 +4833,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>178</v>
       </c>
@@ -4820,7 +4853,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>178</v>
       </c>
@@ -4840,7 +4873,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>178</v>
       </c>
@@ -4860,7 +4893,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>178</v>
       </c>
@@ -4892,7 +4925,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
         <v>178</v>
       </c>
@@ -4924,7 +4957,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
         <v>178</v>
       </c>
@@ -4956,7 +4989,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10">
       <c r="A102" t="s">
         <v>178</v>
       </c>
@@ -4988,7 +5021,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10">
       <c r="A103" t="s">
         <v>178</v>
       </c>
@@ -5020,7 +5053,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10">
       <c r="A104" t="s">
         <v>178</v>
       </c>
@@ -5052,7 +5085,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10">
       <c r="A105" t="s">
         <v>178</v>
       </c>
@@ -5084,7 +5117,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10">
       <c r="A106" t="s">
         <v>178</v>
       </c>
@@ -5116,7 +5149,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10">
       <c r="A107" t="s">
         <v>178</v>
       </c>
@@ -5148,7 +5181,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10">
       <c r="A108" t="s">
         <v>178</v>
       </c>
@@ -5180,7 +5213,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10">
       <c r="A109" t="s">
         <v>178</v>
       </c>
@@ -5212,7 +5245,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10">
       <c r="A110" t="s">
         <v>178</v>
       </c>
@@ -5244,7 +5277,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10">
       <c r="A111" t="s">
         <v>178</v>
       </c>
@@ -5276,7 +5309,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10">
       <c r="A112" t="s">
         <v>178</v>
       </c>
@@ -5308,7 +5341,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>178</v>
       </c>
@@ -5340,7 +5373,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>178</v>
       </c>
@@ -5372,7 +5405,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>178</v>
       </c>
@@ -5404,7 +5437,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10">
       <c r="A116" t="s">
         <v>178</v>
       </c>
@@ -5436,7 +5469,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>178</v>
       </c>
@@ -5468,7 +5501,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>178</v>
       </c>
@@ -5500,7 +5533,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10">
       <c r="A119" t="s">
         <v>178</v>
       </c>
@@ -5532,7 +5565,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10">
       <c r="A120" t="s">
         <v>178</v>
       </c>
@@ -5564,7 +5597,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10">
       <c r="A121" t="s">
         <v>178</v>
       </c>
@@ -5596,7 +5629,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10">
       <c r="A122" t="s">
         <v>178</v>
       </c>
@@ -5628,7 +5661,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10">
       <c r="A123" t="s">
         <v>178</v>
       </c>
@@ -5660,7 +5693,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10">
       <c r="A124" t="s">
         <v>178</v>
       </c>
@@ -5699,6 +5732,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5706,19 +5744,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" customWidth="1"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="73.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -5732,7 +5769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>183</v>
       </c>
@@ -5743,7 +5780,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -5761,6 +5798,11 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5768,21 +5810,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
       <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125"/>
-    <col min="3" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="3" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -5805,7 +5845,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>183</v>
       </c>
@@ -5829,7 +5869,7 @@
         <v>GEP00004_01A1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>183</v>
       </c>
@@ -5853,7 +5893,7 @@
         <v>GEP00004_01A2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -5877,7 +5917,7 @@
         <v>GEP00004_01A3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -5901,7 +5941,7 @@
         <v>GEP00004_01A4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>183</v>
       </c>
@@ -5925,7 +5965,7 @@
         <v>GEP00004_01A5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>183</v>
       </c>
@@ -5949,7 +5989,7 @@
         <v>GEP00004_01A6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>183</v>
       </c>
@@ -5973,7 +6013,7 @@
         <v>GEP00004_01A7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>183</v>
       </c>
@@ -5997,7 +6037,7 @@
         <v>GEP00004_01A8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>183</v>
       </c>
@@ -6021,7 +6061,7 @@
         <v>GEP00004_01A9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>183</v>
       </c>
@@ -6045,7 +6085,7 @@
         <v>GEP00004_01A10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>183</v>
       </c>
@@ -6069,7 +6109,7 @@
         <v>GEP00004_01A11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>183</v>
       </c>
@@ -6093,7 +6133,7 @@
         <v>GEP00004_01A12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>183</v>
       </c>
@@ -6117,7 +6157,7 @@
         <v>GEP00004_01B1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>183</v>
       </c>
@@ -6141,7 +6181,7 @@
         <v>GEP00004_01B2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>183</v>
       </c>
@@ -6165,7 +6205,7 @@
         <v>GEP00004_01B3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>183</v>
       </c>
@@ -6189,7 +6229,7 @@
         <v>GEP00004_01B4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>183</v>
       </c>
@@ -6213,7 +6253,7 @@
         <v>GEP00004_01B5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>183</v>
       </c>
@@ -6237,7 +6277,7 @@
         <v>GEP00004_01B6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>183</v>
       </c>
@@ -6261,7 +6301,7 @@
         <v>GEP00004_01B7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>183</v>
       </c>
@@ -6285,7 +6325,7 @@
         <v>GEP00004_01B8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>183</v>
       </c>
@@ -6309,7 +6349,7 @@
         <v>GEP00004_01B9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -6333,7 +6373,7 @@
         <v>GEP00004_01B10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>183</v>
       </c>
@@ -6357,7 +6397,7 @@
         <v>GEP00004_01B11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>183</v>
       </c>
@@ -6381,7 +6421,7 @@
         <v>GEP00004_01B12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>183</v>
       </c>
@@ -6405,7 +6445,7 @@
         <v>GEP00004_01C1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>183</v>
       </c>
@@ -6429,7 +6469,7 @@
         <v>GEP00004_01C2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>183</v>
       </c>
@@ -6453,7 +6493,7 @@
         <v>GEP00004_01C3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>183</v>
       </c>
@@ -6477,7 +6517,7 @@
         <v>GEP00004_01C4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>183</v>
       </c>
@@ -6501,7 +6541,7 @@
         <v>GEP00004_01C5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>183</v>
       </c>
@@ -6525,7 +6565,7 @@
         <v>GEP00004_01C6</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>183</v>
       </c>
@@ -6549,7 +6589,7 @@
         <v>GEP00004_01C7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -6573,7 +6613,7 @@
         <v>GEP00004_01C8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>183</v>
       </c>
@@ -6597,7 +6637,7 @@
         <v>GEP00004_01C9</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>183</v>
       </c>
@@ -6621,7 +6661,7 @@
         <v>GEP00004_01C10</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>183</v>
       </c>
@@ -6645,7 +6685,7 @@
         <v>GEP00004_01C11</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -6669,7 +6709,7 @@
         <v>GEP00004_01C12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -6693,7 +6733,7 @@
         <v>GEP00004_01D1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>183</v>
       </c>
@@ -6717,7 +6757,7 @@
         <v>GEP00004_01D2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -6741,7 +6781,7 @@
         <v>GEP00004_01D3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>183</v>
       </c>
@@ -6765,7 +6805,7 @@
         <v>GEP00004_01D4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -6789,7 +6829,7 @@
         <v>GEP00004_01D5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>183</v>
       </c>
@@ -6813,7 +6853,7 @@
         <v>GEP00004_01D6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>183</v>
       </c>
@@ -6837,7 +6877,7 @@
         <v>GEP00004_01D7</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>183</v>
       </c>
@@ -6861,7 +6901,7 @@
         <v>GEP00004_01D8</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>183</v>
       </c>
@@ -6885,7 +6925,7 @@
         <v>GEP00004_01D9</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>183</v>
       </c>
@@ -6909,7 +6949,7 @@
         <v>GEP00004_01D10</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>183</v>
       </c>
@@ -6933,7 +6973,7 @@
         <v>GEP00004_01D11</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>183</v>
       </c>
@@ -6957,7 +6997,7 @@
         <v>GEP00004_01D12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>183</v>
       </c>
@@ -6981,7 +7021,7 @@
         <v>GEP00004_01E1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>183</v>
       </c>
@@ -7005,7 +7045,7 @@
         <v>GEP00004_01E2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>183</v>
       </c>
@@ -7029,7 +7069,7 @@
         <v>GEP00004_01E3</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>183</v>
       </c>
@@ -7053,7 +7093,7 @@
         <v>GEP00004_01E4</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>183</v>
       </c>
@@ -7077,7 +7117,7 @@
         <v>GEP00004_01E5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>183</v>
       </c>
@@ -7101,7 +7141,7 @@
         <v>GEP00004_01E6</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>183</v>
       </c>
@@ -7125,7 +7165,7 @@
         <v>GEP00004_01E7</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>183</v>
       </c>
@@ -7149,7 +7189,7 @@
         <v>GEP00004_01E8</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>183</v>
       </c>
@@ -7173,7 +7213,7 @@
         <v>GEP00004_01E9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>183</v>
       </c>
@@ -7197,7 +7237,7 @@
         <v>GEP00004_01E10</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>183</v>
       </c>
@@ -7221,7 +7261,7 @@
         <v>GEP00004_01E11</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>183</v>
       </c>
@@ -7245,7 +7285,7 @@
         <v>GEP00004_01E12</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>183</v>
       </c>
@@ -7269,7 +7309,7 @@
         <v>GEP00004_01F1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>183</v>
       </c>
@@ -7293,7 +7333,7 @@
         <v>GEP00004_01F2</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>183</v>
       </c>
@@ -7317,7 +7357,7 @@
         <v>GEP00004_01F3</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>183</v>
       </c>
@@ -7341,7 +7381,7 @@
         <v>GEP00004_01F4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>183</v>
       </c>
@@ -7365,7 +7405,7 @@
         <v>GEP00004_01F5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>183</v>
       </c>
@@ -7389,7 +7429,7 @@
         <v>GEP00004_01F6</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>183</v>
       </c>
@@ -7413,7 +7453,7 @@
         <v>GEP00004_01F7</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>183</v>
       </c>
@@ -7437,7 +7477,7 @@
         <v>GEP00004_01F8</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>183</v>
       </c>
@@ -7461,7 +7501,7 @@
         <v>GEP00004_01F9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>183</v>
       </c>
@@ -7485,7 +7525,7 @@
         <v>GEP00004_01F10</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>183</v>
       </c>
@@ -7509,7 +7549,7 @@
         <v>GEP00004_01F11</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>183</v>
       </c>
@@ -7533,7 +7573,7 @@
         <v>GEP00004_01F12</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>183</v>
       </c>
@@ -7557,7 +7597,7 @@
         <v>GEP00004_01G1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>183</v>
       </c>
@@ -7581,7 +7621,7 @@
         <v>GEP00004_01G2</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -7605,7 +7645,7 @@
         <v>GEP00004_01G3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>183</v>
       </c>
@@ -7629,7 +7669,7 @@
         <v>GEP00004_01G4</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>183</v>
       </c>
@@ -7653,7 +7693,7 @@
         <v>GEP00004_01G5</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>183</v>
       </c>
@@ -7677,7 +7717,7 @@
         <v>GEP00004_01G6</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>183</v>
       </c>
@@ -7701,7 +7741,7 @@
         <v>GEP00004_01G7</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -7725,7 +7765,7 @@
         <v>GEP00004_01G8</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>183</v>
       </c>
@@ -7749,7 +7789,7 @@
         <v>GEP00004_01G9</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>183</v>
       </c>
@@ -7773,7 +7813,7 @@
         <v>GEP00004_01G10</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>183</v>
       </c>
@@ -7797,7 +7837,7 @@
         <v>GEP00004_01G11</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>183</v>
       </c>
@@ -7821,7 +7861,7 @@
         <v>GEP00004_01G12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>183</v>
       </c>
@@ -7845,7 +7885,7 @@
         <v>GEP00004_01H1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>183</v>
       </c>
@@ -7869,7 +7909,7 @@
         <v>GEP00004_01H2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>183</v>
       </c>
@@ -7893,7 +7933,7 @@
         <v>GEP00004_01H3</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>183</v>
       </c>
@@ -7917,7 +7957,7 @@
         <v>GEP00004_01H4</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>183</v>
       </c>
@@ -7941,7 +7981,7 @@
         <v>GEP00004_01H5</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>183</v>
       </c>
@@ -7965,7 +8005,7 @@
         <v>GEP00004_01H6</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>183</v>
       </c>
@@ -7989,7 +8029,7 @@
         <v>GEP00004_01H7</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>183</v>
       </c>
@@ -8013,7 +8053,7 @@
         <v>GEP00004_01H8</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -8037,7 +8077,7 @@
         <v>GEP00004_01H9</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>183</v>
       </c>
@@ -8061,7 +8101,7 @@
         <v>GEP00004_01H10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>183</v>
       </c>
@@ -8085,7 +8125,7 @@
         <v>GEP00004_01H11</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>183</v>
       </c>
@@ -8109,7 +8149,7 @@
         <v>GEP00004_01H12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>184</v>
       </c>
@@ -8133,7 +8173,7 @@
         <v>GEP00004_02A5</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>184</v>
       </c>
@@ -8157,7 +8197,7 @@
         <v>GEP00004_02A6</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>184</v>
       </c>
@@ -8181,7 +8221,7 @@
         <v>GEP00004_02A7</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>184</v>
       </c>
@@ -8205,7 +8245,7 @@
         <v>GEP00004_02A8</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>184</v>
       </c>
@@ -8229,7 +8269,7 @@
         <v>GEP00004_02B5</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>184</v>
       </c>
@@ -8253,7 +8293,7 @@
         <v>GEP00004_02B6</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>184</v>
       </c>
@@ -8277,7 +8317,7 @@
         <v>GEP00004_02B7</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>184</v>
       </c>
@@ -8301,7 +8341,7 @@
         <v>GEP00004_02B8</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106" t="s">
         <v>184</v>
       </c>
@@ -8325,7 +8365,7 @@
         <v>GEP00004_02C5</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7">
       <c r="A107" t="s">
         <v>184</v>
       </c>
@@ -8349,7 +8389,7 @@
         <v>GEP00004_02C6</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108" t="s">
         <v>184</v>
       </c>
@@ -8373,7 +8413,7 @@
         <v>GEP00004_02C7</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7">
       <c r="A109" t="s">
         <v>184</v>
       </c>
@@ -8397,7 +8437,7 @@
         <v>GEP00004_02C8</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110" t="s">
         <v>184</v>
       </c>
@@ -8421,7 +8461,7 @@
         <v>GEP00004_02D5</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7">
       <c r="A111" t="s">
         <v>184</v>
       </c>
@@ -8445,7 +8485,7 @@
         <v>GEP00004_02D6</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7">
       <c r="A112" t="s">
         <v>184</v>
       </c>
@@ -8469,7 +8509,7 @@
         <v>GEP00004_02D7</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7">
       <c r="A113" t="s">
         <v>184</v>
       </c>
@@ -8493,7 +8533,7 @@
         <v>GEP00004_02E5</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7">
       <c r="A114" t="s">
         <v>184</v>
       </c>
@@ -8517,7 +8557,7 @@
         <v>GEP00004_02E6</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7">
       <c r="A115" t="s">
         <v>184</v>
       </c>
@@ -8541,7 +8581,7 @@
         <v>GEP00004_02E7</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
         <v>184</v>
       </c>
@@ -8565,7 +8605,7 @@
         <v>GEP00004_02F5</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
         <v>184</v>
       </c>
@@ -8589,7 +8629,7 @@
         <v>GEP00004_02F6</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
         <v>184</v>
       </c>
@@ -8613,7 +8653,7 @@
         <v>GEP00004_02F7</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7">
       <c r="A119" t="s">
         <v>184</v>
       </c>
@@ -8637,7 +8677,7 @@
         <v>GEP00004_02G5</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7">
       <c r="A120" t="s">
         <v>184</v>
       </c>
@@ -8661,7 +8701,7 @@
         <v>GEP00004_02G6</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
         <v>184</v>
       </c>
@@ -8685,7 +8725,7 @@
         <v>GEP00004_02G7</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7">
       <c r="A122" t="s">
         <v>184</v>
       </c>
@@ -8709,7 +8749,7 @@
         <v>GEP00004_02H5</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7">
       <c r="A123" t="s">
         <v>184</v>
       </c>
@@ -8733,7 +8773,7 @@
         <v>GEP00004_02H6</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7">
       <c r="A124" t="s">
         <v>184</v>
       </c>
@@ -8764,5 +8804,10 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove link to genome from cell line, revert to genome GRCh38.p7 in projects 4 & 7, comment out pool field on cell line and fix ForeignKey name to genome
</commit_message>
<xml_diff>
--- a/data/GEP00004/GEP00004_ARID1B.xlsx
+++ b/data/GEP00004/GEP00004_ARID1B.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="4280" windowWidth="25600" windowHeight="16060" tabRatio="649" activeTab="7"/>
+    <workbookView xWindow="34280" yWindow="5220" windowWidth="25600" windowHeight="16060" tabRatio="649" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Plate" sheetId="7" r:id="rId7"/>
     <sheet name="SequencingLibrary" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -964,10 +964,10 @@
     <t>negative</t>
   </si>
   <si>
-    <t>GRCh37.p13</t>
-  </si>
-  <si>
     <t>non-fixed cells</t>
+  </si>
+  <si>
+    <t>GRCh38.p7</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1341,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1443,7 +1443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1497,7 +1497,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>65</v>
@@ -5820,7 +5820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
@@ -5863,7 +5863,7 @@
         <v>73</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D2" t="s">
         <v>307</v>
@@ -5887,7 +5887,7 @@
         <v>74</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D3" t="s">
         <v>307</v>
@@ -5911,7 +5911,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D4" t="s">
         <v>307</v>
@@ -5935,7 +5935,7 @@
         <v>76</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D5" t="s">
         <v>307</v>
@@ -5959,7 +5959,7 @@
         <v>77</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D6" t="s">
         <v>307</v>
@@ -5983,7 +5983,7 @@
         <v>78</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D7" t="s">
         <v>307</v>
@@ -6007,7 +6007,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D8" t="s">
         <v>307</v>
@@ -6031,7 +6031,7 @@
         <v>80</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D9" t="s">
         <v>307</v>
@@ -6055,7 +6055,7 @@
         <v>81</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D10" t="s">
         <v>307</v>
@@ -6079,7 +6079,7 @@
         <v>82</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D11" t="s">
         <v>307</v>
@@ -6103,7 +6103,7 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D12" t="s">
         <v>307</v>
@@ -6127,7 +6127,7 @@
         <v>84</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D13" t="s">
         <v>307</v>
@@ -6151,7 +6151,7 @@
         <v>85</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D14" t="s">
         <v>307</v>
@@ -6175,7 +6175,7 @@
         <v>86</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D15" t="s">
         <v>307</v>
@@ -6199,7 +6199,7 @@
         <v>87</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D16" t="s">
         <v>307</v>
@@ -6223,7 +6223,7 @@
         <v>88</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D17" t="s">
         <v>307</v>
@@ -6247,7 +6247,7 @@
         <v>89</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D18" t="s">
         <v>307</v>
@@ -6271,7 +6271,7 @@
         <v>90</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D19" t="s">
         <v>307</v>
@@ -6295,7 +6295,7 @@
         <v>91</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D20" t="s">
         <v>307</v>
@@ -6319,7 +6319,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D21" t="s">
         <v>307</v>
@@ -6343,7 +6343,7 @@
         <v>93</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D22" t="s">
         <v>307</v>
@@ -6367,7 +6367,7 @@
         <v>94</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D23" t="s">
         <v>307</v>
@@ -6391,7 +6391,7 @@
         <v>95</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D24" t="s">
         <v>307</v>
@@ -6415,7 +6415,7 @@
         <v>96</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D25" t="s">
         <v>307</v>
@@ -6439,7 +6439,7 @@
         <v>97</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D26" t="s">
         <v>307</v>
@@ -6463,7 +6463,7 @@
         <v>98</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D27" t="s">
         <v>307</v>
@@ -6487,7 +6487,7 @@
         <v>99</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D28" t="s">
         <v>307</v>
@@ -6511,7 +6511,7 @@
         <v>100</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D29" t="s">
         <v>307</v>
@@ -6535,7 +6535,7 @@
         <v>101</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D30" t="s">
         <v>307</v>
@@ -6559,7 +6559,7 @@
         <v>102</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D31" t="s">
         <v>307</v>
@@ -6583,7 +6583,7 @@
         <v>103</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D32" t="s">
         <v>307</v>
@@ -6607,7 +6607,7 @@
         <v>104</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D33" t="s">
         <v>307</v>
@@ -6631,7 +6631,7 @@
         <v>105</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D34" t="s">
         <v>307</v>
@@ -6655,7 +6655,7 @@
         <v>106</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D35" t="s">
         <v>307</v>
@@ -6679,7 +6679,7 @@
         <v>107</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D36" t="s">
         <v>307</v>
@@ -6703,7 +6703,7 @@
         <v>108</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D37" t="s">
         <v>307</v>
@@ -6727,7 +6727,7 @@
         <v>109</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D38" t="s">
         <v>307</v>
@@ -6751,7 +6751,7 @@
         <v>110</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D39" t="s">
         <v>307</v>
@@ -6775,7 +6775,7 @@
         <v>111</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D40" t="s">
         <v>307</v>
@@ -6799,7 +6799,7 @@
         <v>112</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D41" t="s">
         <v>307</v>
@@ -6823,7 +6823,7 @@
         <v>113</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D42" t="s">
         <v>307</v>
@@ -6847,7 +6847,7 @@
         <v>114</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D43" t="s">
         <v>307</v>
@@ -6871,7 +6871,7 @@
         <v>115</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D44" t="s">
         <v>307</v>
@@ -6895,7 +6895,7 @@
         <v>116</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D45" t="s">
         <v>307</v>
@@ -6919,7 +6919,7 @@
         <v>117</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D46" t="s">
         <v>307</v>
@@ -6943,7 +6943,7 @@
         <v>118</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D47" t="s">
         <v>307</v>
@@ -6967,7 +6967,7 @@
         <v>119</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D48" t="s">
         <v>307</v>
@@ -6991,7 +6991,7 @@
         <v>120</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D49" t="s">
         <v>307</v>
@@ -7015,7 +7015,7 @@
         <v>121</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D50" t="s">
         <v>307</v>
@@ -7039,7 +7039,7 @@
         <v>122</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D51" t="s">
         <v>307</v>
@@ -7063,7 +7063,7 @@
         <v>123</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D52" t="s">
         <v>307</v>
@@ -7087,7 +7087,7 @@
         <v>124</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D53" t="s">
         <v>307</v>
@@ -7111,7 +7111,7 @@
         <v>125</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D54" t="s">
         <v>307</v>
@@ -7135,7 +7135,7 @@
         <v>126</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D55" t="s">
         <v>307</v>
@@ -7159,7 +7159,7 @@
         <v>127</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D56" t="s">
         <v>307</v>
@@ -7183,7 +7183,7 @@
         <v>128</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D57" t="s">
         <v>307</v>
@@ -7207,7 +7207,7 @@
         <v>129</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D58" t="s">
         <v>307</v>
@@ -7231,7 +7231,7 @@
         <v>130</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D59" t="s">
         <v>307</v>
@@ -7255,7 +7255,7 @@
         <v>131</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D60" t="s">
         <v>307</v>
@@ -7279,7 +7279,7 @@
         <v>132</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D61" t="s">
         <v>307</v>
@@ -7303,7 +7303,7 @@
         <v>133</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D62" t="s">
         <v>307</v>
@@ -7327,7 +7327,7 @@
         <v>134</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D63" t="s">
         <v>307</v>
@@ -7351,7 +7351,7 @@
         <v>135</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D64" t="s">
         <v>307</v>
@@ -7375,7 +7375,7 @@
         <v>136</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D65" t="s">
         <v>307</v>
@@ -7399,7 +7399,7 @@
         <v>137</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D66" t="s">
         <v>307</v>
@@ -7423,7 +7423,7 @@
         <v>138</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D67" t="s">
         <v>307</v>
@@ -7447,7 +7447,7 @@
         <v>139</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D68" t="s">
         <v>307</v>
@@ -7471,7 +7471,7 @@
         <v>140</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D69" t="s">
         <v>307</v>
@@ -7495,7 +7495,7 @@
         <v>141</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D70" t="s">
         <v>307</v>
@@ -7519,7 +7519,7 @@
         <v>142</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D71" t="s">
         <v>307</v>
@@ -7543,7 +7543,7 @@
         <v>143</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D72" t="s">
         <v>307</v>
@@ -7567,7 +7567,7 @@
         <v>144</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D73" t="s">
         <v>307</v>
@@ -7591,7 +7591,7 @@
         <v>145</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D74" t="s">
         <v>307</v>
@@ -7615,7 +7615,7 @@
         <v>146</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D75" t="s">
         <v>307</v>
@@ -7639,7 +7639,7 @@
         <v>147</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D76" t="s">
         <v>307</v>
@@ -7663,7 +7663,7 @@
         <v>148</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D77" t="s">
         <v>307</v>
@@ -7687,7 +7687,7 @@
         <v>149</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D78" t="s">
         <v>307</v>
@@ -7711,7 +7711,7 @@
         <v>150</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D79" t="s">
         <v>307</v>
@@ -7735,7 +7735,7 @@
         <v>151</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D80" t="s">
         <v>307</v>
@@ -7759,7 +7759,7 @@
         <v>152</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D81" t="s">
         <v>307</v>
@@ -7783,7 +7783,7 @@
         <v>153</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D82" t="s">
         <v>307</v>
@@ -7807,7 +7807,7 @@
         <v>154</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D83" t="s">
         <v>307</v>
@@ -7831,7 +7831,7 @@
         <v>155</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D84" t="s">
         <v>307</v>
@@ -7855,7 +7855,7 @@
         <v>156</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D85" t="s">
         <v>307</v>
@@ -7879,7 +7879,7 @@
         <v>157</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D86" t="s">
         <v>307</v>
@@ -7903,7 +7903,7 @@
         <v>158</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D87" t="s">
         <v>307</v>
@@ -7927,7 +7927,7 @@
         <v>159</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D88" t="s">
         <v>307</v>
@@ -7951,7 +7951,7 @@
         <v>160</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D89" t="s">
         <v>307</v>
@@ -7975,7 +7975,7 @@
         <v>161</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D90" t="s">
         <v>307</v>
@@ -7999,7 +7999,7 @@
         <v>162</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D91" t="s">
         <v>307</v>
@@ -8023,7 +8023,7 @@
         <v>163</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D92" t="s">
         <v>307</v>
@@ -8047,7 +8047,7 @@
         <v>164</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D93" t="s">
         <v>307</v>
@@ -8071,7 +8071,7 @@
         <v>165</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D94" t="s">
         <v>307</v>
@@ -8095,7 +8095,7 @@
         <v>166</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D95" t="s">
         <v>307</v>
@@ -8119,7 +8119,7 @@
         <v>167</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D96" t="s">
         <v>307</v>
@@ -8143,7 +8143,7 @@
         <v>168</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D97" t="s">
         <v>307</v>
@@ -8167,7 +8167,7 @@
         <v>77</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D98" t="s">
         <v>307</v>
@@ -8191,7 +8191,7 @@
         <v>78</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D99" t="s">
         <v>307</v>
@@ -8215,7 +8215,7 @@
         <v>79</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D100" t="s">
         <v>307</v>
@@ -8239,7 +8239,7 @@
         <v>80</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D101" t="s">
         <v>307</v>
@@ -8263,7 +8263,7 @@
         <v>89</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D102" t="s">
         <v>307</v>
@@ -8287,7 +8287,7 @@
         <v>90</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D103" t="s">
         <v>307</v>
@@ -8311,7 +8311,7 @@
         <v>91</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D104" t="s">
         <v>307</v>
@@ -8335,7 +8335,7 @@
         <v>92</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D105" t="s">
         <v>307</v>
@@ -8359,7 +8359,7 @@
         <v>101</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D106" t="s">
         <v>307</v>
@@ -8383,7 +8383,7 @@
         <v>102</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D107" t="s">
         <v>307</v>
@@ -8407,7 +8407,7 @@
         <v>103</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D108" t="s">
         <v>307</v>
@@ -8431,7 +8431,7 @@
         <v>104</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D109" t="s">
         <v>307</v>
@@ -8455,7 +8455,7 @@
         <v>113</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D110" t="s">
         <v>307</v>
@@ -8479,7 +8479,7 @@
         <v>114</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D111" t="s">
         <v>307</v>
@@ -8503,7 +8503,7 @@
         <v>115</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D112" t="s">
         <v>307</v>
@@ -8527,7 +8527,7 @@
         <v>125</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D113" t="s">
         <v>307</v>
@@ -8551,7 +8551,7 @@
         <v>126</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D114" t="s">
         <v>307</v>
@@ -8575,7 +8575,7 @@
         <v>127</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D115" t="s">
         <v>307</v>
@@ -8599,7 +8599,7 @@
         <v>137</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D116" t="s">
         <v>307</v>
@@ -8623,7 +8623,7 @@
         <v>138</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D117" t="s">
         <v>307</v>
@@ -8647,7 +8647,7 @@
         <v>139</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D118" t="s">
         <v>307</v>
@@ -8671,7 +8671,7 @@
         <v>149</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D119" t="s">
         <v>307</v>
@@ -8695,7 +8695,7 @@
         <v>150</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D120" t="s">
         <v>307</v>
@@ -8719,7 +8719,7 @@
         <v>151</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D121" t="s">
         <v>307</v>
@@ -8743,7 +8743,7 @@
         <v>161</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D122" t="s">
         <v>307</v>
@@ -8767,7 +8767,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D123" t="s">
         <v>307</v>
@@ -8791,7 +8791,7 @@
         <v>163</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D124" t="s">
         <v>307</v>

</xml_diff>

<commit_message>
rename file, version should not be added to filename, neither space or any special characters
</commit_message>
<xml_diff>
--- a/data/GEP00004/GEP00004_ARID1B.xlsx
+++ b/data/GEP00004/GEP00004_ARID1B.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smith04\Desktop\NGS final submission\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34280" yWindow="5220" windowWidth="25600" windowHeight="16060" tabRatio="649" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13170" tabRatio="649" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
     <sheet name="Plate" sheetId="7" r:id="rId7"/>
     <sheet name="SequencingLibrary" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -967,14 +972,14 @@
     <t>non-fixed cells</t>
   </si>
   <si>
-    <t>GRCh38.p7</t>
+    <t>GRCh38</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1341,7 +1346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1352,15 +1357,15 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="6" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="9" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="6" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1443,15 +1448,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1544,13 +1549,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1645,11 +1650,11 @@
       <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1689,21 +1694,21 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="15.5" customWidth="1"/>
-    <col min="11" max="14" width="14.1640625" customWidth="1"/>
-    <col min="15" max="16" width="14.83203125" customWidth="1"/>
-    <col min="17" max="18" width="31.6640625" customWidth="1"/>
-    <col min="19" max="21" width="14.83203125" customWidth="1"/>
-    <col min="22" max="22" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="16" width="14.85546875" customWidth="1"/>
+    <col min="17" max="18" width="31.7109375" customWidth="1"/>
+    <col min="19" max="21" width="14.85546875" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -1885,18 +1890,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="1" max="2" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1965,7 +1970,7 @@
         <v>169</v>
       </c>
       <c r="E3">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
         <v>170</v>
@@ -1997,7 +2002,7 @@
         <v>169</v>
       </c>
       <c r="E4">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>170</v>
@@ -2029,7 +2034,7 @@
         <v>169</v>
       </c>
       <c r="E5">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
         <v>170</v>
@@ -2061,7 +2066,7 @@
         <v>169</v>
       </c>
       <c r="E6">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
         <v>170</v>
@@ -2093,7 +2098,7 @@
         <v>169</v>
       </c>
       <c r="E7">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
         <v>170</v>
@@ -2125,7 +2130,7 @@
         <v>169</v>
       </c>
       <c r="E8">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
         <v>170</v>
@@ -2157,7 +2162,7 @@
         <v>169</v>
       </c>
       <c r="E9">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
         <v>170</v>
@@ -2189,7 +2194,7 @@
         <v>169</v>
       </c>
       <c r="E10">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>170</v>
@@ -2221,7 +2226,7 @@
         <v>169</v>
       </c>
       <c r="E11">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
         <v>170</v>
@@ -2273,7 +2278,7 @@
         <v>169</v>
       </c>
       <c r="E13">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
         <v>170</v>
@@ -2305,7 +2310,7 @@
         <v>169</v>
       </c>
       <c r="E14">
-        <v>82.1</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>170</v>
@@ -2337,7 +2342,7 @@
         <v>169</v>
       </c>
       <c r="E15">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
         <v>170</v>
@@ -2369,7 +2374,7 @@
         <v>169</v>
       </c>
       <c r="E16">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
         <v>170</v>
@@ -2401,7 +2406,7 @@
         <v>169</v>
       </c>
       <c r="E17">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
         <v>170</v>
@@ -2433,7 +2438,7 @@
         <v>169</v>
       </c>
       <c r="E18">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
         <v>170</v>
@@ -2465,7 +2470,7 @@
         <v>169</v>
       </c>
       <c r="E19">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>170</v>
@@ -2497,7 +2502,7 @@
         <v>169</v>
       </c>
       <c r="E20">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>170</v>
@@ -2529,7 +2534,7 @@
         <v>169</v>
       </c>
       <c r="E21">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
         <v>170</v>
@@ -2561,7 +2566,7 @@
         <v>169</v>
       </c>
       <c r="E22">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
         <v>170</v>
@@ -2593,7 +2598,7 @@
         <v>169</v>
       </c>
       <c r="E23">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
         <v>170</v>
@@ -2645,7 +2650,7 @@
         <v>169</v>
       </c>
       <c r="E25">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
         <v>170</v>
@@ -2677,7 +2682,7 @@
         <v>169</v>
       </c>
       <c r="E26">
-        <v>82.1</v>
+        <v>1</v>
       </c>
       <c r="F26" t="s">
         <v>170</v>
@@ -2709,7 +2714,7 @@
         <v>169</v>
       </c>
       <c r="E27">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F27" t="s">
         <v>170</v>
@@ -2741,7 +2746,7 @@
         <v>169</v>
       </c>
       <c r="E28">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F28" t="s">
         <v>170</v>
@@ -2773,7 +2778,7 @@
         <v>169</v>
       </c>
       <c r="E29">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F29" t="s">
         <v>170</v>
@@ -2805,7 +2810,7 @@
         <v>169</v>
       </c>
       <c r="E30">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F30" t="s">
         <v>170</v>
@@ -2837,7 +2842,7 @@
         <v>169</v>
       </c>
       <c r="E31">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
         <v>170</v>
@@ -2869,7 +2874,7 @@
         <v>169</v>
       </c>
       <c r="E32">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
         <v>170</v>
@@ -2901,7 +2906,7 @@
         <v>169</v>
       </c>
       <c r="E33">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
         <v>170</v>
@@ -2933,7 +2938,7 @@
         <v>169</v>
       </c>
       <c r="E34">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
         <v>170</v>
@@ -2965,7 +2970,7 @@
         <v>169</v>
       </c>
       <c r="E35">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F35" t="s">
         <v>170</v>
@@ -3017,7 +3022,7 @@
         <v>169</v>
       </c>
       <c r="E37">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F37" t="s">
         <v>170</v>
@@ -3049,7 +3054,7 @@
         <v>169</v>
       </c>
       <c r="E38">
-        <v>82.1</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
         <v>170</v>
@@ -3081,7 +3086,7 @@
         <v>169</v>
       </c>
       <c r="E39">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F39" t="s">
         <v>170</v>
@@ -3113,7 +3118,7 @@
         <v>169</v>
       </c>
       <c r="E40">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F40" t="s">
         <v>170</v>
@@ -3145,7 +3150,7 @@
         <v>169</v>
       </c>
       <c r="E41">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F41" t="s">
         <v>170</v>
@@ -3177,7 +3182,7 @@
         <v>169</v>
       </c>
       <c r="E42">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F42" t="s">
         <v>170</v>
@@ -3209,7 +3214,7 @@
         <v>169</v>
       </c>
       <c r="E43">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F43" t="s">
         <v>170</v>
@@ -3241,7 +3246,7 @@
         <v>169</v>
       </c>
       <c r="E44">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
         <v>170</v>
@@ -3273,7 +3278,7 @@
         <v>169</v>
       </c>
       <c r="E45">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
         <v>170</v>
@@ -3305,7 +3310,7 @@
         <v>169</v>
       </c>
       <c r="E46">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F46" t="s">
         <v>170</v>
@@ -3337,7 +3342,7 @@
         <v>169</v>
       </c>
       <c r="E47">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F47" t="s">
         <v>170</v>
@@ -3389,7 +3394,7 @@
         <v>169</v>
       </c>
       <c r="E49">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F49" t="s">
         <v>170</v>
@@ -3421,7 +3426,7 @@
         <v>169</v>
       </c>
       <c r="E50">
-        <v>82.1</v>
+        <v>1</v>
       </c>
       <c r="F50" t="s">
         <v>170</v>
@@ -3453,7 +3458,7 @@
         <v>169</v>
       </c>
       <c r="E51">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F51" t="s">
         <v>170</v>
@@ -3485,7 +3490,7 @@
         <v>169</v>
       </c>
       <c r="E52">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F52" t="s">
         <v>170</v>
@@ -3517,7 +3522,7 @@
         <v>169</v>
       </c>
       <c r="E53">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F53" t="s">
         <v>170</v>
@@ -3549,7 +3554,7 @@
         <v>169</v>
       </c>
       <c r="E54">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F54" t="s">
         <v>170</v>
@@ -3581,7 +3586,7 @@
         <v>169</v>
       </c>
       <c r="E55">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F55" t="s">
         <v>170</v>
@@ -3613,7 +3618,7 @@
         <v>169</v>
       </c>
       <c r="E56">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F56" t="s">
         <v>170</v>
@@ -3645,7 +3650,7 @@
         <v>169</v>
       </c>
       <c r="E57">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F57" t="s">
         <v>170</v>
@@ -3677,7 +3682,7 @@
         <v>169</v>
       </c>
       <c r="E58">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F58" t="s">
         <v>170</v>
@@ -3709,7 +3714,7 @@
         <v>169</v>
       </c>
       <c r="E59">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F59" t="s">
         <v>170</v>
@@ -3761,7 +3766,7 @@
         <v>169</v>
       </c>
       <c r="E61">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F61" t="s">
         <v>170</v>
@@ -3793,7 +3798,7 @@
         <v>169</v>
       </c>
       <c r="E62">
-        <v>82.1</v>
+        <v>1</v>
       </c>
       <c r="F62" t="s">
         <v>170</v>
@@ -3825,7 +3830,7 @@
         <v>169</v>
       </c>
       <c r="E63">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F63" t="s">
         <v>170</v>
@@ -3857,7 +3862,7 @@
         <v>169</v>
       </c>
       <c r="E64">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F64" t="s">
         <v>170</v>
@@ -3889,7 +3894,7 @@
         <v>169</v>
       </c>
       <c r="E65">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F65" t="s">
         <v>170</v>
@@ -3921,7 +3926,7 @@
         <v>169</v>
       </c>
       <c r="E66">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F66" t="s">
         <v>170</v>
@@ -3953,7 +3958,7 @@
         <v>169</v>
       </c>
       <c r="E67">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F67" t="s">
         <v>170</v>
@@ -3985,7 +3990,7 @@
         <v>169</v>
       </c>
       <c r="E68">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F68" t="s">
         <v>170</v>
@@ -4017,7 +4022,7 @@
         <v>169</v>
       </c>
       <c r="E69">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F69" t="s">
         <v>170</v>
@@ -4049,7 +4054,7 @@
         <v>169</v>
       </c>
       <c r="E70">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F70" t="s">
         <v>170</v>
@@ -4081,7 +4086,7 @@
         <v>169</v>
       </c>
       <c r="E71">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F71" t="s">
         <v>170</v>
@@ -4133,7 +4138,7 @@
         <v>169</v>
       </c>
       <c r="E73">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F73" t="s">
         <v>170</v>
@@ -4165,7 +4170,7 @@
         <v>169</v>
       </c>
       <c r="E74">
-        <v>82.1</v>
+        <v>1</v>
       </c>
       <c r="F74" t="s">
         <v>170</v>
@@ -4197,7 +4202,7 @@
         <v>169</v>
       </c>
       <c r="E75">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F75" t="s">
         <v>170</v>
@@ -4229,7 +4234,7 @@
         <v>169</v>
       </c>
       <c r="E76">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F76" t="s">
         <v>170</v>
@@ -4261,7 +4266,7 @@
         <v>169</v>
       </c>
       <c r="E77">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F77" t="s">
         <v>170</v>
@@ -4293,7 +4298,7 @@
         <v>169</v>
       </c>
       <c r="E78">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F78" t="s">
         <v>170</v>
@@ -4325,7 +4330,7 @@
         <v>169</v>
       </c>
       <c r="E79">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F79" t="s">
         <v>170</v>
@@ -4357,7 +4362,7 @@
         <v>169</v>
       </c>
       <c r="E80">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F80" t="s">
         <v>170</v>
@@ -4389,7 +4394,7 @@
         <v>169</v>
       </c>
       <c r="E81">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F81" t="s">
         <v>170</v>
@@ -4421,7 +4426,7 @@
         <v>169</v>
       </c>
       <c r="E82">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F82" t="s">
         <v>170</v>
@@ -4453,7 +4458,7 @@
         <v>169</v>
       </c>
       <c r="E83">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F83" t="s">
         <v>170</v>
@@ -4505,7 +4510,7 @@
         <v>169</v>
       </c>
       <c r="E85">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F85" t="s">
         <v>170</v>
@@ -4537,7 +4542,7 @@
         <v>169</v>
       </c>
       <c r="E86">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F86" t="s">
         <v>170</v>
@@ -4569,7 +4574,7 @@
         <v>169</v>
       </c>
       <c r="E87">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F87" t="s">
         <v>170</v>
@@ -4601,7 +4606,7 @@
         <v>169</v>
       </c>
       <c r="E88">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F88" t="s">
         <v>170</v>
@@ -4633,7 +4638,7 @@
         <v>169</v>
       </c>
       <c r="E89">
-        <v>82.3</v>
+        <v>3</v>
       </c>
       <c r="F89" t="s">
         <v>170</v>
@@ -4665,7 +4670,7 @@
         <v>169</v>
       </c>
       <c r="E90">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F90" t="s">
         <v>170</v>
@@ -4697,7 +4702,7 @@
         <v>169</v>
       </c>
       <c r="E91">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F91" t="s">
         <v>170</v>
@@ -4729,7 +4734,7 @@
         <v>169</v>
       </c>
       <c r="E92">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F92" t="s">
         <v>170</v>
@@ -4761,7 +4766,7 @@
         <v>169</v>
       </c>
       <c r="E93">
-        <v>84.1</v>
+        <v>1</v>
       </c>
       <c r="F93" t="s">
         <v>170</v>
@@ -4793,7 +4798,7 @@
         <v>169</v>
       </c>
       <c r="E94">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F94" t="s">
         <v>170</v>
@@ -4825,7 +4830,7 @@
         <v>169</v>
       </c>
       <c r="E95">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F95" t="s">
         <v>170</v>
@@ -4917,7 +4922,7 @@
         <v>169</v>
       </c>
       <c r="E99">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F99" t="s">
         <v>170</v>
@@ -4949,7 +4954,7 @@
         <v>169</v>
       </c>
       <c r="E100">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F100" t="s">
         <v>170</v>
@@ -5013,7 +5018,7 @@
         <v>169</v>
       </c>
       <c r="E102">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F102" t="s">
         <v>170</v>
@@ -5045,7 +5050,7 @@
         <v>169</v>
       </c>
       <c r="E103">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F103" t="s">
         <v>170</v>
@@ -5077,7 +5082,7 @@
         <v>169</v>
       </c>
       <c r="E104">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F104" t="s">
         <v>170</v>
@@ -5141,7 +5146,7 @@
         <v>169</v>
       </c>
       <c r="E106">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F106" t="s">
         <v>170</v>
@@ -5173,7 +5178,7 @@
         <v>169</v>
       </c>
       <c r="E107">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F107" t="s">
         <v>170</v>
@@ -5205,7 +5210,7 @@
         <v>169</v>
       </c>
       <c r="E108">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F108" t="s">
         <v>170</v>
@@ -5269,7 +5274,7 @@
         <v>169</v>
       </c>
       <c r="E110">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F110" t="s">
         <v>170</v>
@@ -5301,7 +5306,7 @@
         <v>169</v>
       </c>
       <c r="E111">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F111" t="s">
         <v>170</v>
@@ -5333,7 +5338,7 @@
         <v>169</v>
       </c>
       <c r="E112">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F112" t="s">
         <v>170</v>
@@ -5365,7 +5370,7 @@
         <v>169</v>
       </c>
       <c r="E113">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F113" t="s">
         <v>170</v>
@@ -5397,7 +5402,7 @@
         <v>169</v>
       </c>
       <c r="E114">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F114" t="s">
         <v>170</v>
@@ -5429,7 +5434,7 @@
         <v>169</v>
       </c>
       <c r="E115">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F115" t="s">
         <v>170</v>
@@ -5461,7 +5466,7 @@
         <v>169</v>
       </c>
       <c r="E116">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F116" t="s">
         <v>170</v>
@@ -5493,7 +5498,7 @@
         <v>169</v>
       </c>
       <c r="E117">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F117" t="s">
         <v>170</v>
@@ -5557,7 +5562,7 @@
         <v>169</v>
       </c>
       <c r="E119">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F119" t="s">
         <v>170</v>
@@ -5589,7 +5594,7 @@
         <v>169</v>
       </c>
       <c r="E120">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F120" t="s">
         <v>170</v>
@@ -5653,7 +5658,7 @@
         <v>169</v>
       </c>
       <c r="E122">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F122" t="s">
         <v>170</v>
@@ -5685,7 +5690,7 @@
         <v>169</v>
       </c>
       <c r="E123">
-        <v>84.2</v>
+        <v>2</v>
       </c>
       <c r="F123" t="s">
         <v>170</v>
@@ -5758,11 +5763,11 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="73.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5820,16 +5825,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="3" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="3" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5855,7 +5860,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" t="s">
         <v>179</v>
       </c>
@@ -5879,7 +5884,7 @@
         <v>GEP00004_01A1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -5903,7 +5908,7 @@
         <v>GEP00004_01A2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16">
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -5927,7 +5932,7 @@
         <v>GEP00004_01A3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16">
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -5951,7 +5956,7 @@
         <v>GEP00004_01A4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16">
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" t="s">
         <v>179</v>
       </c>
@@ -5975,7 +5980,7 @@
         <v>GEP00004_01A5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16">
+    <row r="7" spans="1:7" ht="15">
       <c r="A7" t="s">
         <v>179</v>
       </c>
@@ -5999,7 +6004,7 @@
         <v>GEP00004_01A6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16">
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" t="s">
         <v>179</v>
       </c>
@@ -6023,7 +6028,7 @@
         <v>GEP00004_01A7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16">
+    <row r="9" spans="1:7" ht="15">
       <c r="A9" t="s">
         <v>179</v>
       </c>
@@ -6047,7 +6052,7 @@
         <v>GEP00004_01A8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16">
+    <row r="10" spans="1:7" ht="15">
       <c r="A10" t="s">
         <v>179</v>
       </c>
@@ -6071,7 +6076,7 @@
         <v>GEP00004_01A9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16">
+    <row r="11" spans="1:7" ht="15">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -6095,7 +6100,7 @@
         <v>GEP00004_01A10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16">
+    <row r="12" spans="1:7" ht="15">
       <c r="A12" t="s">
         <v>179</v>
       </c>
@@ -6119,7 +6124,7 @@
         <v>GEP00004_01A11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16">
+    <row r="13" spans="1:7" ht="15">
       <c r="A13" t="s">
         <v>179</v>
       </c>
@@ -6143,7 +6148,7 @@
         <v>GEP00004_01A12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16">
+    <row r="14" spans="1:7" ht="15">
       <c r="A14" t="s">
         <v>179</v>
       </c>
@@ -6167,7 +6172,7 @@
         <v>GEP00004_01B1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16">
+    <row r="15" spans="1:7" ht="15">
       <c r="A15" t="s">
         <v>179</v>
       </c>
@@ -6191,7 +6196,7 @@
         <v>GEP00004_01B2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16">
+    <row r="16" spans="1:7" ht="15">
       <c r="A16" t="s">
         <v>179</v>
       </c>
@@ -6215,7 +6220,7 @@
         <v>GEP00004_01B3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16">
+    <row r="17" spans="1:7" ht="15">
       <c r="A17" t="s">
         <v>179</v>
       </c>
@@ -6239,7 +6244,7 @@
         <v>GEP00004_01B4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16">
+    <row r="18" spans="1:7" ht="15">
       <c r="A18" t="s">
         <v>179</v>
       </c>
@@ -6263,7 +6268,7 @@
         <v>GEP00004_01B5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16">
+    <row r="19" spans="1:7" ht="15">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -6287,7 +6292,7 @@
         <v>GEP00004_01B6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16">
+    <row r="20" spans="1:7" ht="15">
       <c r="A20" t="s">
         <v>179</v>
       </c>
@@ -6311,7 +6316,7 @@
         <v>GEP00004_01B7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16">
+    <row r="21" spans="1:7" ht="15">
       <c r="A21" t="s">
         <v>179</v>
       </c>
@@ -6335,7 +6340,7 @@
         <v>GEP00004_01B8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16">
+    <row r="22" spans="1:7" ht="15">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -6359,7 +6364,7 @@
         <v>GEP00004_01B9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16">
+    <row r="23" spans="1:7" ht="15">
       <c r="A23" t="s">
         <v>179</v>
       </c>
@@ -6383,7 +6388,7 @@
         <v>GEP00004_01B10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16">
+    <row r="24" spans="1:7" ht="15">
       <c r="A24" t="s">
         <v>179</v>
       </c>
@@ -6407,7 +6412,7 @@
         <v>GEP00004_01B11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16">
+    <row r="25" spans="1:7" ht="15">
       <c r="A25" t="s">
         <v>179</v>
       </c>
@@ -6431,7 +6436,7 @@
         <v>GEP00004_01B12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16">
+    <row r="26" spans="1:7" ht="15">
       <c r="A26" t="s">
         <v>179</v>
       </c>
@@ -6455,7 +6460,7 @@
         <v>GEP00004_01C1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16">
+    <row r="27" spans="1:7" ht="15">
       <c r="A27" t="s">
         <v>179</v>
       </c>
@@ -6479,7 +6484,7 @@
         <v>GEP00004_01C2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16">
+    <row r="28" spans="1:7" ht="15">
       <c r="A28" t="s">
         <v>179</v>
       </c>
@@ -6503,7 +6508,7 @@
         <v>GEP00004_01C3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16">
+    <row r="29" spans="1:7" ht="15">
       <c r="A29" t="s">
         <v>179</v>
       </c>
@@ -6527,7 +6532,7 @@
         <v>GEP00004_01C4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16">
+    <row r="30" spans="1:7" ht="15">
       <c r="A30" t="s">
         <v>179</v>
       </c>
@@ -6551,7 +6556,7 @@
         <v>GEP00004_01C5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16">
+    <row r="31" spans="1:7" ht="15">
       <c r="A31" t="s">
         <v>179</v>
       </c>
@@ -6575,7 +6580,7 @@
         <v>GEP00004_01C6</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16">
+    <row r="32" spans="1:7" ht="15">
       <c r="A32" t="s">
         <v>179</v>
       </c>
@@ -6599,7 +6604,7 @@
         <v>GEP00004_01C7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16">
+    <row r="33" spans="1:7" ht="15">
       <c r="A33" t="s">
         <v>179</v>
       </c>
@@ -6623,7 +6628,7 @@
         <v>GEP00004_01C8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16">
+    <row r="34" spans="1:7" ht="15">
       <c r="A34" t="s">
         <v>179</v>
       </c>
@@ -6647,7 +6652,7 @@
         <v>GEP00004_01C9</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16">
+    <row r="35" spans="1:7" ht="15">
       <c r="A35" t="s">
         <v>179</v>
       </c>
@@ -6671,7 +6676,7 @@
         <v>GEP00004_01C10</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16">
+    <row r="36" spans="1:7" ht="15">
       <c r="A36" t="s">
         <v>179</v>
       </c>
@@ -6695,7 +6700,7 @@
         <v>GEP00004_01C11</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16">
+    <row r="37" spans="1:7" ht="15">
       <c r="A37" t="s">
         <v>179</v>
       </c>
@@ -6719,7 +6724,7 @@
         <v>GEP00004_01C12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16">
+    <row r="38" spans="1:7" ht="15">
       <c r="A38" t="s">
         <v>179</v>
       </c>
@@ -6743,7 +6748,7 @@
         <v>GEP00004_01D1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16">
+    <row r="39" spans="1:7" ht="15">
       <c r="A39" t="s">
         <v>179</v>
       </c>
@@ -6767,7 +6772,7 @@
         <v>GEP00004_01D2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="16">
+    <row r="40" spans="1:7" ht="15">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -6791,7 +6796,7 @@
         <v>GEP00004_01D3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16">
+    <row r="41" spans="1:7" ht="15">
       <c r="A41" t="s">
         <v>179</v>
       </c>
@@ -6815,7 +6820,7 @@
         <v>GEP00004_01D4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="16">
+    <row r="42" spans="1:7" ht="15">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -6839,7 +6844,7 @@
         <v>GEP00004_01D5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="16">
+    <row r="43" spans="1:7" ht="15">
       <c r="A43" t="s">
         <v>179</v>
       </c>
@@ -6863,7 +6868,7 @@
         <v>GEP00004_01D6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="16">
+    <row r="44" spans="1:7" ht="15">
       <c r="A44" t="s">
         <v>179</v>
       </c>
@@ -6887,7 +6892,7 @@
         <v>GEP00004_01D7</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="16">
+    <row r="45" spans="1:7" ht="15">
       <c r="A45" t="s">
         <v>179</v>
       </c>
@@ -6911,7 +6916,7 @@
         <v>GEP00004_01D8</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="16">
+    <row r="46" spans="1:7" ht="15">
       <c r="A46" t="s">
         <v>179</v>
       </c>
@@ -6935,7 +6940,7 @@
         <v>GEP00004_01D9</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="16">
+    <row r="47" spans="1:7" ht="15">
       <c r="A47" t="s">
         <v>179</v>
       </c>
@@ -6959,7 +6964,7 @@
         <v>GEP00004_01D10</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="16">
+    <row r="48" spans="1:7" ht="15">
       <c r="A48" t="s">
         <v>179</v>
       </c>
@@ -6983,7 +6988,7 @@
         <v>GEP00004_01D11</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16">
+    <row r="49" spans="1:7" ht="15">
       <c r="A49" t="s">
         <v>179</v>
       </c>
@@ -7007,7 +7012,7 @@
         <v>GEP00004_01D12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16">
+    <row r="50" spans="1:7" ht="15">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -7031,7 +7036,7 @@
         <v>GEP00004_01E1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16">
+    <row r="51" spans="1:7" ht="15">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -7055,7 +7060,7 @@
         <v>GEP00004_01E2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="16">
+    <row r="52" spans="1:7" ht="15">
       <c r="A52" t="s">
         <v>179</v>
       </c>
@@ -7079,7 +7084,7 @@
         <v>GEP00004_01E3</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="16">
+    <row r="53" spans="1:7" ht="15">
       <c r="A53" t="s">
         <v>179</v>
       </c>
@@ -7103,7 +7108,7 @@
         <v>GEP00004_01E4</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="16">
+    <row r="54" spans="1:7" ht="15">
       <c r="A54" t="s">
         <v>179</v>
       </c>
@@ -7127,7 +7132,7 @@
         <v>GEP00004_01E5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="16">
+    <row r="55" spans="1:7" ht="15">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -7151,7 +7156,7 @@
         <v>GEP00004_01E6</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="16">
+    <row r="56" spans="1:7" ht="15">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -7175,7 +7180,7 @@
         <v>GEP00004_01E7</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16">
+    <row r="57" spans="1:7" ht="15">
       <c r="A57" t="s">
         <v>179</v>
       </c>
@@ -7199,7 +7204,7 @@
         <v>GEP00004_01E8</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="16">
+    <row r="58" spans="1:7" ht="15">
       <c r="A58" t="s">
         <v>179</v>
       </c>
@@ -7223,7 +7228,7 @@
         <v>GEP00004_01E9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="16">
+    <row r="59" spans="1:7" ht="15">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -7247,7 +7252,7 @@
         <v>GEP00004_01E10</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="16">
+    <row r="60" spans="1:7" ht="15">
       <c r="A60" t="s">
         <v>179</v>
       </c>
@@ -7271,7 +7276,7 @@
         <v>GEP00004_01E11</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="16">
+    <row r="61" spans="1:7" ht="15">
       <c r="A61" t="s">
         <v>179</v>
       </c>
@@ -7295,7 +7300,7 @@
         <v>GEP00004_01E12</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="16">
+    <row r="62" spans="1:7" ht="15">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -7319,7 +7324,7 @@
         <v>GEP00004_01F1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="16">
+    <row r="63" spans="1:7" ht="15">
       <c r="A63" t="s">
         <v>179</v>
       </c>
@@ -7343,7 +7348,7 @@
         <v>GEP00004_01F2</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16">
+    <row r="64" spans="1:7" ht="15">
       <c r="A64" t="s">
         <v>179</v>
       </c>
@@ -7367,7 +7372,7 @@
         <v>GEP00004_01F3</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="16">
+    <row r="65" spans="1:7" ht="15">
       <c r="A65" t="s">
         <v>179</v>
       </c>
@@ -7391,7 +7396,7 @@
         <v>GEP00004_01F4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="16">
+    <row r="66" spans="1:7" ht="15">
       <c r="A66" t="s">
         <v>179</v>
       </c>
@@ -7415,7 +7420,7 @@
         <v>GEP00004_01F5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="16">
+    <row r="67" spans="1:7" ht="15">
       <c r="A67" t="s">
         <v>179</v>
       </c>
@@ -7439,7 +7444,7 @@
         <v>GEP00004_01F6</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="16">
+    <row r="68" spans="1:7" ht="15">
       <c r="A68" t="s">
         <v>179</v>
       </c>
@@ -7463,7 +7468,7 @@
         <v>GEP00004_01F7</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="16">
+    <row r="69" spans="1:7" ht="15">
       <c r="A69" t="s">
         <v>179</v>
       </c>
@@ -7487,7 +7492,7 @@
         <v>GEP00004_01F8</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="16">
+    <row r="70" spans="1:7" ht="15">
       <c r="A70" t="s">
         <v>179</v>
       </c>
@@ -7511,7 +7516,7 @@
         <v>GEP00004_01F9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="16">
+    <row r="71" spans="1:7" ht="15">
       <c r="A71" t="s">
         <v>179</v>
       </c>
@@ -7535,7 +7540,7 @@
         <v>GEP00004_01F10</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="16">
+    <row r="72" spans="1:7" ht="15">
       <c r="A72" t="s">
         <v>179</v>
       </c>
@@ -7559,7 +7564,7 @@
         <v>GEP00004_01F11</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="16">
+    <row r="73" spans="1:7" ht="15">
       <c r="A73" t="s">
         <v>179</v>
       </c>
@@ -7583,7 +7588,7 @@
         <v>GEP00004_01F12</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="16">
+    <row r="74" spans="1:7" ht="15">
       <c r="A74" t="s">
         <v>179</v>
       </c>
@@ -7607,7 +7612,7 @@
         <v>GEP00004_01G1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="16">
+    <row r="75" spans="1:7" ht="15">
       <c r="A75" t="s">
         <v>179</v>
       </c>
@@ -7631,7 +7636,7 @@
         <v>GEP00004_01G2</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="16">
+    <row r="76" spans="1:7" ht="15">
       <c r="A76" t="s">
         <v>179</v>
       </c>
@@ -7655,7 +7660,7 @@
         <v>GEP00004_01G3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="16">
+    <row r="77" spans="1:7" ht="15">
       <c r="A77" t="s">
         <v>179</v>
       </c>
@@ -7679,7 +7684,7 @@
         <v>GEP00004_01G4</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="16">
+    <row r="78" spans="1:7" ht="15">
       <c r="A78" t="s">
         <v>179</v>
       </c>
@@ -7703,7 +7708,7 @@
         <v>GEP00004_01G5</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="16">
+    <row r="79" spans="1:7" ht="15">
       <c r="A79" t="s">
         <v>179</v>
       </c>
@@ -7727,7 +7732,7 @@
         <v>GEP00004_01G6</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="16">
+    <row r="80" spans="1:7" ht="15">
       <c r="A80" t="s">
         <v>179</v>
       </c>
@@ -7751,7 +7756,7 @@
         <v>GEP00004_01G7</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="16">
+    <row r="81" spans="1:7" ht="15">
       <c r="A81" t="s">
         <v>179</v>
       </c>
@@ -7775,7 +7780,7 @@
         <v>GEP00004_01G8</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="16">
+    <row r="82" spans="1:7" ht="15">
       <c r="A82" t="s">
         <v>179</v>
       </c>
@@ -7799,7 +7804,7 @@
         <v>GEP00004_01G9</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="16">
+    <row r="83" spans="1:7" ht="15">
       <c r="A83" t="s">
         <v>179</v>
       </c>
@@ -7823,7 +7828,7 @@
         <v>GEP00004_01G10</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="16">
+    <row r="84" spans="1:7" ht="15">
       <c r="A84" t="s">
         <v>179</v>
       </c>
@@ -7847,7 +7852,7 @@
         <v>GEP00004_01G11</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="16">
+    <row r="85" spans="1:7" ht="15">
       <c r="A85" t="s">
         <v>179</v>
       </c>
@@ -7871,7 +7876,7 @@
         <v>GEP00004_01G12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="16">
+    <row r="86" spans="1:7" ht="15">
       <c r="A86" t="s">
         <v>179</v>
       </c>
@@ -7895,7 +7900,7 @@
         <v>GEP00004_01H1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="16">
+    <row r="87" spans="1:7" ht="15">
       <c r="A87" t="s">
         <v>179</v>
       </c>
@@ -7919,7 +7924,7 @@
         <v>GEP00004_01H2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="16">
+    <row r="88" spans="1:7" ht="15">
       <c r="A88" t="s">
         <v>179</v>
       </c>
@@ -7943,7 +7948,7 @@
         <v>GEP00004_01H3</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="16">
+    <row r="89" spans="1:7" ht="15">
       <c r="A89" t="s">
         <v>179</v>
       </c>
@@ -7967,7 +7972,7 @@
         <v>GEP00004_01H4</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="16">
+    <row r="90" spans="1:7" ht="15">
       <c r="A90" t="s">
         <v>179</v>
       </c>
@@ -7991,7 +7996,7 @@
         <v>GEP00004_01H5</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="16">
+    <row r="91" spans="1:7" ht="15">
       <c r="A91" t="s">
         <v>179</v>
       </c>
@@ -8015,7 +8020,7 @@
         <v>GEP00004_01H6</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="16">
+    <row r="92" spans="1:7" ht="15">
       <c r="A92" t="s">
         <v>179</v>
       </c>
@@ -8039,7 +8044,7 @@
         <v>GEP00004_01H7</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="16">
+    <row r="93" spans="1:7" ht="15">
       <c r="A93" t="s">
         <v>179</v>
       </c>
@@ -8063,7 +8068,7 @@
         <v>GEP00004_01H8</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="16">
+    <row r="94" spans="1:7" ht="15">
       <c r="A94" t="s">
         <v>179</v>
       </c>
@@ -8087,7 +8092,7 @@
         <v>GEP00004_01H9</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="16">
+    <row r="95" spans="1:7" ht="15">
       <c r="A95" t="s">
         <v>179</v>
       </c>
@@ -8111,7 +8116,7 @@
         <v>GEP00004_01H10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="16">
+    <row r="96" spans="1:7" ht="15">
       <c r="A96" t="s">
         <v>179</v>
       </c>
@@ -8135,7 +8140,7 @@
         <v>GEP00004_01H11</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="16">
+    <row r="97" spans="1:7" ht="15">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -8159,7 +8164,7 @@
         <v>GEP00004_01H12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="16">
+    <row r="98" spans="1:7" ht="15">
       <c r="A98" t="s">
         <v>180</v>
       </c>
@@ -8183,7 +8188,7 @@
         <v>GEP00004_02A5</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="16">
+    <row r="99" spans="1:7" ht="15">
       <c r="A99" t="s">
         <v>180</v>
       </c>
@@ -8207,7 +8212,7 @@
         <v>GEP00004_02A6</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="16">
+    <row r="100" spans="1:7" ht="15">
       <c r="A100" t="s">
         <v>180</v>
       </c>
@@ -8231,7 +8236,7 @@
         <v>GEP00004_02A7</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="16">
+    <row r="101" spans="1:7" ht="15">
       <c r="A101" t="s">
         <v>180</v>
       </c>
@@ -8255,7 +8260,7 @@
         <v>GEP00004_02A8</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="16">
+    <row r="102" spans="1:7" ht="15">
       <c r="A102" t="s">
         <v>180</v>
       </c>
@@ -8279,7 +8284,7 @@
         <v>GEP00004_02B5</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="16">
+    <row r="103" spans="1:7" ht="15">
       <c r="A103" t="s">
         <v>180</v>
       </c>
@@ -8303,7 +8308,7 @@
         <v>GEP00004_02B6</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="16">
+    <row r="104" spans="1:7" ht="15">
       <c r="A104" t="s">
         <v>180</v>
       </c>
@@ -8327,7 +8332,7 @@
         <v>GEP00004_02B7</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="16">
+    <row r="105" spans="1:7" ht="15">
       <c r="A105" t="s">
         <v>180</v>
       </c>
@@ -8351,7 +8356,7 @@
         <v>GEP00004_02B8</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="16">
+    <row r="106" spans="1:7" ht="15">
       <c r="A106" t="s">
         <v>180</v>
       </c>
@@ -8375,7 +8380,7 @@
         <v>GEP00004_02C5</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="16">
+    <row r="107" spans="1:7" ht="15">
       <c r="A107" t="s">
         <v>180</v>
       </c>
@@ -8399,7 +8404,7 @@
         <v>GEP00004_02C6</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="16">
+    <row r="108" spans="1:7" ht="15">
       <c r="A108" t="s">
         <v>180</v>
       </c>
@@ -8423,7 +8428,7 @@
         <v>GEP00004_02C7</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="16">
+    <row r="109" spans="1:7" ht="15">
       <c r="A109" t="s">
         <v>180</v>
       </c>
@@ -8447,7 +8452,7 @@
         <v>GEP00004_02C8</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="16">
+    <row r="110" spans="1:7" ht="15">
       <c r="A110" t="s">
         <v>180</v>
       </c>
@@ -8471,7 +8476,7 @@
         <v>GEP00004_02D5</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="16">
+    <row r="111" spans="1:7" ht="15">
       <c r="A111" t="s">
         <v>180</v>
       </c>
@@ -8495,7 +8500,7 @@
         <v>GEP00004_02D6</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="16">
+    <row r="112" spans="1:7" ht="15">
       <c r="A112" t="s">
         <v>180</v>
       </c>
@@ -8519,7 +8524,7 @@
         <v>GEP00004_02D7</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="16">
+    <row r="113" spans="1:7" ht="15">
       <c r="A113" t="s">
         <v>180</v>
       </c>
@@ -8543,7 +8548,7 @@
         <v>GEP00004_02E5</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="16">
+    <row r="114" spans="1:7" ht="15">
       <c r="A114" t="s">
         <v>180</v>
       </c>
@@ -8567,7 +8572,7 @@
         <v>GEP00004_02E6</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="16">
+    <row r="115" spans="1:7" ht="15">
       <c r="A115" t="s">
         <v>180</v>
       </c>
@@ -8591,7 +8596,7 @@
         <v>GEP00004_02E7</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="16">
+    <row r="116" spans="1:7" ht="15">
       <c r="A116" t="s">
         <v>180</v>
       </c>
@@ -8615,7 +8620,7 @@
         <v>GEP00004_02F5</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="16">
+    <row r="117" spans="1:7" ht="15">
       <c r="A117" t="s">
         <v>180</v>
       </c>
@@ -8639,7 +8644,7 @@
         <v>GEP00004_02F6</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="16">
+    <row r="118" spans="1:7" ht="15">
       <c r="A118" t="s">
         <v>180</v>
       </c>
@@ -8663,7 +8668,7 @@
         <v>GEP00004_02F7</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="16">
+    <row r="119" spans="1:7" ht="15">
       <c r="A119" t="s">
         <v>180</v>
       </c>
@@ -8687,7 +8692,7 @@
         <v>GEP00004_02G5</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="16">
+    <row r="120" spans="1:7" ht="15">
       <c r="A120" t="s">
         <v>180</v>
       </c>
@@ -8711,7 +8716,7 @@
         <v>GEP00004_02G6</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="16">
+    <row r="121" spans="1:7" ht="15">
       <c r="A121" t="s">
         <v>180</v>
       </c>
@@ -8735,7 +8740,7 @@
         <v>GEP00004_02G7</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="16">
+    <row r="122" spans="1:7" ht="15">
       <c r="A122" t="s">
         <v>180</v>
       </c>
@@ -8759,7 +8764,7 @@
         <v>GEP00004_02H5</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="16">
+    <row r="123" spans="1:7" ht="15">
       <c r="A123" t="s">
         <v>180</v>
       </c>
@@ -8783,7 +8788,7 @@
         <v>GEP00004_02H6</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="16">
+    <row r="124" spans="1:7" ht="15">
       <c r="A124" t="s">
         <v>180</v>
       </c>

</xml_diff>